<commit_message>
add other columns to sens analysis
</commit_message>
<xml_diff>
--- a/results/easq-sensitivity-analysis.xlsx
+++ b/results/easq-sensitivity-analysis.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -361,7 +361,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>dom</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -371,44 +371,54 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>N_no4</t>
+          <t>N</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>N_all</t>
+          <t>q1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>point.diff_no4</t>
+          <t>q3</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>point.diff_all</t>
+          <t>pred.q1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Pval_no4</t>
+          <t>pred.q3</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Pval_all</t>
+          <t>point.diff</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>sensitivity</t>
+          <t>lb.diff</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ub.diff</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pval</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_no4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -420,28 +430,34 @@
         <v>764</v>
       </c>
       <c r="D2">
-        <v>765</v>
+        <v>0.230348825</v>
       </c>
       <c r="E2">
+        <v>0.8012372000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.0419345670332736</v>
+      </c>
+      <c r="G2">
+        <v>0.04299751975423131</v>
+      </c>
+      <c r="H2">
         <v>0.001062952720957721</v>
       </c>
-      <c r="F2">
-        <v>0.08492172999772614</v>
-      </c>
-      <c r="G2">
+      <c r="I2">
+        <v>-0.03714448939531297</v>
+      </c>
+      <c r="J2">
+        <v>0.03927039483722841</v>
+      </c>
+      <c r="K2">
         <v>0.9604688695318725</v>
-      </c>
-      <c r="H2">
-        <v>0.3329959493332269</v>
-      </c>
-      <c r="I2">
-        <v>0.9874831480589694</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_no4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -453,28 +469,34 @@
         <v>759</v>
       </c>
       <c r="D3">
-        <v>765</v>
+        <v>0.23013515</v>
       </c>
       <c r="E3">
+        <v>0.8013165</v>
+      </c>
+      <c r="F3">
+        <v>0.1325259159874605</v>
+      </c>
+      <c r="G3">
+        <v>0.1235274546259792</v>
+      </c>
+      <c r="H3">
         <v>-0.008998461361481271</v>
       </c>
-      <c r="F3">
-        <v>-0.05162075746174589</v>
-      </c>
-      <c r="G3">
+      <c r="I3">
+        <v>-0.04043766501103746</v>
+      </c>
+      <c r="J3">
+        <v>0.02244074228807492</v>
+      </c>
+      <c r="K3">
         <v>0.5867563997725677</v>
-      </c>
-      <c r="H3">
-        <v>0.6640093382022003</v>
-      </c>
-      <c r="I3">
-        <v>0.8256813382068313</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_no4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -486,28 +508,34 @@
         <v>761</v>
       </c>
       <c r="D4">
-        <v>765</v>
+        <v>0.2305625</v>
       </c>
       <c r="E4">
+        <v>0.8014751</v>
+      </c>
+      <c r="F4">
+        <v>0.03892189728541484</v>
+      </c>
+      <c r="G4">
+        <v>0.02309521865777314</v>
+      </c>
+      <c r="H4">
         <v>-0.0158266786276417</v>
       </c>
-      <c r="F4">
-        <v>0.003734835513529286</v>
-      </c>
-      <c r="G4">
+      <c r="I4">
+        <v>-0.07652230803457477</v>
+      </c>
+      <c r="J4">
+        <v>0.04486895077929137</v>
+      </c>
+      <c r="K4">
         <v>0.6218203181949693</v>
-      </c>
-      <c r="H4">
-        <v>0.8866704771970065</v>
-      </c>
-      <c r="I4">
-        <v>5.237583842798488</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_no4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -519,1210 +547,2992 @@
         <v>761</v>
       </c>
       <c r="D5">
-        <v>765</v>
+        <v>0.2305625</v>
       </c>
       <c r="E5">
+        <v>0.8011579</v>
+      </c>
+      <c r="F5">
+        <v>-0.07566214564481774</v>
+      </c>
+      <c r="G5">
+        <v>-0.07261175568379917</v>
+      </c>
+      <c r="H5">
         <v>0.003050389961018559</v>
       </c>
-      <c r="F5">
-        <v>0.01175860716711812</v>
-      </c>
-      <c r="G5">
+      <c r="I5">
+        <v>-0.04670956379135138</v>
+      </c>
+      <c r="J5">
+        <v>0.0528103437133885</v>
+      </c>
+      <c r="K5">
         <v>0.9119640817619526</v>
-      </c>
-      <c r="H5">
-        <v>0.6111611180418326</v>
-      </c>
-      <c r="I5">
-        <v>0.7405823736038484</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>aat1</t>
         </is>
       </c>
       <c r="C6">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D6">
-        <v>767</v>
+        <v>0.2297078</v>
       </c>
       <c r="E6">
-        <v>-0.06674069572990476</v>
+        <v>0.8011579</v>
       </c>
       <c r="F6">
-        <v>-0.0624929625997022</v>
+        <v>0.006159270120829587</v>
       </c>
       <c r="G6">
-        <v>0.04938619032521363</v>
+        <v>0.09108100011855573</v>
       </c>
       <c r="H6">
-        <v>0.0699666252065687</v>
+        <v>0.08492172999772614</v>
       </c>
       <c r="I6">
-        <v>-0.06797138355259864</v>
+        <v>-0.08521205619896281</v>
+      </c>
+      <c r="J6">
+        <v>0.2550555161944151</v>
+      </c>
+      <c r="K6">
+        <v>0.3329959493332269</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>aat1</t>
         </is>
       </c>
       <c r="C7">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="D7">
-        <v>767</v>
+        <v>0.2297078</v>
       </c>
       <c r="E7">
-        <v>0.02399166926710282</v>
+        <v>0.8011579</v>
       </c>
       <c r="F7">
-        <v>0.05413253527114577</v>
+        <v>0.1498094796655503</v>
       </c>
       <c r="G7">
-        <v>0.8616626870182504</v>
+        <v>0.0981887222038044</v>
       </c>
       <c r="H7">
-        <v>0.685140600682432</v>
+        <v>-0.05162075746174589</v>
       </c>
       <c r="I7">
-        <v>0.5567976052307477</v>
+        <v>-0.2752888902006794</v>
+      </c>
+      <c r="J7">
+        <v>0.1720473752771876</v>
+      </c>
+      <c r="K7">
+        <v>0.6640093382022003</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>aat1</t>
         </is>
       </c>
       <c r="C8">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="D8">
-        <v>767</v>
+        <v>0.2297078</v>
       </c>
       <c r="E8">
-        <v>-0.1104156867135884</v>
+        <v>0.8011579</v>
       </c>
       <c r="F8">
-        <v>-0.03042802330473879</v>
+        <v>0.01246785780908882</v>
       </c>
       <c r="G8">
-        <v>0.1495256910704528</v>
+        <v>0.01620269332261811</v>
       </c>
       <c r="H8">
-        <v>0.3665363238178662</v>
+        <v>0.003734835513529286</v>
       </c>
       <c r="I8">
-        <v>-2.628749906221892</v>
+        <v>-0.04380016063604917</v>
+      </c>
+      <c r="J8">
+        <v>0.05126983166310774</v>
+      </c>
+      <c r="K8">
+        <v>0.8866704771970065</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>aat1</t>
         </is>
       </c>
       <c r="C9">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="D9">
-        <v>767</v>
+        <v>0.2297078</v>
       </c>
       <c r="E9">
-        <v>-0.09642223039779414</v>
+        <v>0.8011579</v>
       </c>
       <c r="F9">
-        <v>-0.0370512365620911</v>
+        <v>-0.1248406856669598</v>
       </c>
       <c r="G9">
-        <v>0.1904498519366875</v>
+        <v>-0.1130820784998417</v>
       </c>
       <c r="H9">
-        <v>0.2507866464987985</v>
+        <v>0.01175860716711812</v>
       </c>
       <c r="I9">
-        <v>-1.60240249299664</v>
+        <v>-0.03204552435376228</v>
+      </c>
+      <c r="J9">
+        <v>0.05556273868799851</v>
+      </c>
+      <c r="K9">
+        <v>0.6111611180418326</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_no4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>mpo1</t>
         </is>
       </c>
       <c r="C10">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D10">
-        <v>768</v>
+        <v>4285.48065</v>
       </c>
       <c r="E10">
-        <v>0.1396747308864631</v>
+        <v>19821.74375</v>
       </c>
       <c r="F10">
-        <v>0.1574875427849645</v>
+        <v>0.0746215381418108</v>
       </c>
       <c r="G10">
-        <v>0.0697202822196643</v>
+        <v>0.00788084241190604</v>
       </c>
       <c r="H10">
-        <v>0.04573193602110219</v>
+        <v>-0.06674069572990476</v>
       </c>
       <c r="I10">
-        <v>0.1131061643575407</v>
+        <v>-0.1334139115675538</v>
+      </c>
+      <c r="J10">
+        <v>-6.747989225577844e-05</v>
+      </c>
+      <c r="K10">
+        <v>0.04938619032521363</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_no4</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>mpo1</t>
         </is>
       </c>
       <c r="C11">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D11">
-        <v>768</v>
+        <v>4293.9336</v>
       </c>
       <c r="E11">
-        <v>0.05521527881623735</v>
+        <v>19823.689</v>
       </c>
       <c r="F11">
-        <v>0.1035021623789825</v>
+        <v>0.1103240737599749</v>
       </c>
       <c r="G11">
-        <v>0.470259001929198</v>
+        <v>0.1343157430270778</v>
       </c>
       <c r="H11">
-        <v>0.1937881751179691</v>
+        <v>0.02399166926710282</v>
       </c>
       <c r="I11">
-        <v>0.4665301907987042</v>
+        <v>-0.2270636967169867</v>
+      </c>
+      <c r="J11">
+        <v>0.2750470352511924</v>
+      </c>
+      <c r="K11">
+        <v>0.8616626870182504</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_no4</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>mpo1</t>
         </is>
       </c>
       <c r="C12">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D12">
-        <v>768</v>
+        <v>4288.2983</v>
       </c>
       <c r="E12">
-        <v>0.1511486453582206</v>
+        <v>19819.7985</v>
       </c>
       <c r="F12">
-        <v>0.2086005077140167</v>
+        <v>0.06007029351630092</v>
       </c>
       <c r="G12">
-        <v>0.06746107569916637</v>
+        <v>-0.05034539319728752</v>
       </c>
       <c r="H12">
-        <v>0.01524603902894358</v>
+        <v>-0.1104156867135884</v>
       </c>
       <c r="I12">
-        <v>0.2754157359701176</v>
+        <v>-0.2604215903647618</v>
+      </c>
+      <c r="J12">
+        <v>0.03959021693758492</v>
+      </c>
+      <c r="K12">
+        <v>0.1495256910704528</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_no4</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>mpo1</t>
         </is>
       </c>
       <c r="C13">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D13">
-        <v>768</v>
+        <v>4288.2983</v>
       </c>
       <c r="E13">
-        <v>0.1348839056639985</v>
+        <v>19819.7985</v>
       </c>
       <c r="F13">
-        <v>0.2005235301276853</v>
+        <v>-0.04348933699820914</v>
       </c>
       <c r="G13">
-        <v>0.1099988153248812</v>
+        <v>-0.1399115673960033</v>
       </c>
       <c r="H13">
-        <v>0.03886193394109631</v>
+        <v>-0.09642223039779414</v>
       </c>
       <c r="I13">
-        <v>0.3273412572673648</v>
+        <v>-0.240371606666659</v>
+      </c>
+      <c r="J13">
+        <v>0.04752714587107067</v>
+      </c>
+      <c r="K13">
+        <v>0.1904498519366875</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>mpo1</t>
         </is>
       </c>
       <c r="C14">
-        <v>946</v>
+        <v>767</v>
       </c>
       <c r="D14">
-        <v>948</v>
+        <v>4244.6775</v>
       </c>
       <c r="E14">
-        <v>0.03648644438971776</v>
+        <v>19819.7985</v>
       </c>
       <c r="F14">
-        <v>0.07032569010283983</v>
+        <v>0.07546567646788477</v>
       </c>
       <c r="G14">
-        <v>0.7688116603615279</v>
+        <v>0.01297271386818256</v>
       </c>
       <c r="H14">
-        <v>0.5762262133322021</v>
+        <v>-0.0624929625997022</v>
       </c>
       <c r="I14">
-        <v>0.4811790067561043</v>
+        <v>-0.1301798847710062</v>
+      </c>
+      <c r="J14">
+        <v>0.005193959571601833</v>
+      </c>
+      <c r="K14">
+        <v>0.0699666252065687</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>mpo1</t>
         </is>
       </c>
       <c r="C15">
-        <v>944</v>
+        <v>767</v>
       </c>
       <c r="D15">
-        <v>948</v>
+        <v>4244.6775</v>
       </c>
       <c r="E15">
-        <v>-3.817553734995232e-11</v>
+        <v>19819.7985</v>
       </c>
       <c r="F15">
-        <v>-1.322182768828083e-11</v>
+        <v>0.06000436420479705</v>
       </c>
       <c r="G15">
-        <v>0.9999752986052546</v>
+        <v>0.1141368994759428</v>
       </c>
       <c r="H15">
-        <v>0.9999895188837933</v>
+        <v>0.05413253527114577</v>
       </c>
       <c r="I15">
-        <v>-1.887311667492779</v>
+        <v>-0.1964695000191493</v>
+      </c>
+      <c r="J15">
+        <v>0.3047345705614408</v>
+      </c>
+      <c r="K15">
+        <v>0.685140600682432</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>mpo1</t>
         </is>
       </c>
       <c r="C16">
-        <v>943</v>
+        <v>767</v>
       </c>
       <c r="D16">
-        <v>948</v>
+        <v>4244.6775</v>
       </c>
       <c r="E16">
-        <v>9.19530603561722e-07</v>
+        <v>19819.7985</v>
       </c>
       <c r="F16">
-        <v>0.05046051304049208</v>
+        <v>0.03960759996684311</v>
       </c>
       <c r="G16">
-        <v>0.4346082352416721</v>
+        <v>0.009179576662104319</v>
       </c>
       <c r="H16">
-        <v>0.6706885987857295</v>
+        <v>-0.03042802330473879</v>
       </c>
       <c r="I16">
-        <v>0.9999817772244443</v>
+        <v>-0.09564010722536469</v>
+      </c>
+      <c r="J16">
+        <v>0.03478406061588711</v>
+      </c>
+      <c r="K16">
+        <v>0.3665363238178662</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>mpo1</t>
         </is>
       </c>
       <c r="C17">
-        <v>944</v>
+        <v>767</v>
       </c>
       <c r="D17">
-        <v>948</v>
+        <v>4244.6775</v>
       </c>
       <c r="E17">
-        <v>-0.005131777379005095</v>
+        <v>19819.7985</v>
       </c>
       <c r="F17">
-        <v>0.02894133294208512</v>
+        <v>-0.08810203186175078</v>
       </c>
       <c r="G17">
-        <v>0.8292617559056494</v>
+        <v>-0.1251532684238419</v>
       </c>
       <c r="H17">
-        <v>0.801943323732609</v>
+        <v>-0.0370512365620911</v>
       </c>
       <c r="I17">
-        <v>1.177316552394956</v>
+        <v>-0.09992400822925179</v>
+      </c>
+      <c r="J17">
+        <v>0.02582153510506958</v>
+      </c>
+      <c r="K17">
+        <v>0.2507866464987985</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_no4</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>neo1</t>
         </is>
       </c>
       <c r="C18">
-        <v>946</v>
+        <v>767</v>
       </c>
       <c r="D18">
-        <v>948</v>
+        <v>918.33174</v>
       </c>
       <c r="E18">
-        <v>-0.03085221443527438</v>
+        <v>2332.3492</v>
       </c>
       <c r="F18">
-        <v>-0.0281018358588562</v>
+        <v>-0.01122415623964136</v>
       </c>
       <c r="G18">
-        <v>0.1341844510497002</v>
+        <v>0.1284505746468217</v>
       </c>
       <c r="H18">
-        <v>0.1809099304725955</v>
+        <v>0.1396747308864631</v>
       </c>
       <c r="I18">
-        <v>-0.09787184688687907</v>
+        <v>-0.01147623342694096</v>
+      </c>
+      <c r="J18">
+        <v>0.2908256951998672</v>
+      </c>
+      <c r="K18">
+        <v>0.0697202822196643</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_no4</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>neo1</t>
         </is>
       </c>
       <c r="C19">
-        <v>944</v>
+        <v>762</v>
       </c>
       <c r="D19">
-        <v>948</v>
+        <v>919.5907500000001</v>
       </c>
       <c r="E19">
-        <v>0.009620420406050234</v>
+        <v>2332.197125</v>
       </c>
       <c r="F19">
-        <v>0.0114865930097945</v>
+        <v>0.1093381508791628</v>
       </c>
       <c r="G19">
-        <v>0.6277387371373134</v>
+        <v>0.1645534296954001</v>
       </c>
       <c r="H19">
-        <v>0.5448583309930062</v>
+        <v>0.05521527881623735</v>
       </c>
       <c r="I19">
-        <v>0.1624652847152326</v>
+        <v>-0.09161326171673408</v>
+      </c>
+      <c r="J19">
+        <v>0.2020438193492088</v>
+      </c>
+      <c r="K19">
+        <v>0.470259001929198</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_no4</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>neo1</t>
         </is>
       </c>
       <c r="C20">
-        <v>943</v>
+        <v>764</v>
       </c>
       <c r="D20">
-        <v>948</v>
+        <v>920.45225</v>
       </c>
       <c r="E20">
-        <v>-0.004285432713630722</v>
+        <v>2337.7548</v>
       </c>
       <c r="F20">
-        <v>-0.0003677802573873289</v>
+        <v>-0.0181975572609884</v>
       </c>
       <c r="G20">
-        <v>0.8391101309721352</v>
+        <v>0.1329510880972322</v>
       </c>
       <c r="H20">
-        <v>0.986773198790769</v>
+        <v>0.1511486453582206</v>
       </c>
       <c r="I20">
-        <v>-10.65215540408278</v>
+        <v>-0.01109578654878604</v>
+      </c>
+      <c r="J20">
+        <v>0.3133930772652272</v>
+      </c>
+      <c r="K20">
+        <v>0.06746107569916637</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_no4</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>neo1</t>
         </is>
       </c>
       <c r="C21">
-        <v>944</v>
+        <v>764</v>
       </c>
       <c r="D21">
-        <v>948</v>
+        <v>918.74587</v>
       </c>
       <c r="E21">
-        <v>0.08742299827013797</v>
+        <v>2332.2831</v>
       </c>
       <c r="F21">
-        <v>0.009564385164482917</v>
+        <v>-0.1211391162921192</v>
       </c>
       <c r="G21">
-        <v>0.4541203730411344</v>
+        <v>0.0137447893718793</v>
       </c>
       <c r="H21">
-        <v>0.6339435596472874</v>
+        <v>0.1348839056639985</v>
       </c>
       <c r="I21">
-        <v>-8.14047236353267</v>
+        <v>-0.03059512777015372</v>
+      </c>
+      <c r="J21">
+        <v>0.3003629390981506</v>
+      </c>
+      <c r="K21">
+        <v>0.1099988153248812</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>neo1</t>
         </is>
       </c>
       <c r="C22">
-        <v>1338</v>
+        <v>768</v>
       </c>
       <c r="D22">
-        <v>1341</v>
+        <v>917.476365</v>
       </c>
       <c r="E22">
-        <v>0.1569601512246135</v>
+        <v>2332.2831</v>
       </c>
       <c r="F22">
-        <v>0.1500672598950913</v>
+        <v>-0.01547239145993308</v>
       </c>
       <c r="G22">
-        <v>0.09259852070261805</v>
+        <v>0.1420151513250315</v>
       </c>
       <c r="H22">
-        <v>0.119228075809969</v>
+        <v>0.1574875427849645</v>
       </c>
       <c r="I22">
-        <v>-0.04593201298098492</v>
+        <v>0.002725500771095818</v>
+      </c>
+      <c r="J22">
+        <v>0.3122495847988332</v>
+      </c>
+      <c r="K22">
+        <v>0.04573193602110219</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>neo1</t>
         </is>
       </c>
       <c r="C23">
-        <v>1329</v>
+        <v>768</v>
       </c>
       <c r="D23">
-        <v>1341</v>
+        <v>917.476365</v>
       </c>
       <c r="E23">
-        <v>0.06487918076058591</v>
+        <v>2332.2831</v>
       </c>
       <c r="F23">
-        <v>-0.01507026479740493</v>
+        <v>0.08452313430737585</v>
       </c>
       <c r="G23">
-        <v>0.5038169794530788</v>
+        <v>0.1880252966863584</v>
       </c>
       <c r="H23">
-        <v>0.669630718554056</v>
+        <v>0.1035021623789825</v>
       </c>
       <c r="I23">
-        <v>5.305112194960103</v>
+        <v>-0.05215811736958288</v>
+      </c>
+      <c r="J23">
+        <v>0.259162442127548</v>
+      </c>
+      <c r="K23">
+        <v>0.1937881751179691</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>neo1</t>
         </is>
       </c>
       <c r="C24">
-        <v>1332</v>
+        <v>768</v>
       </c>
       <c r="D24">
-        <v>1341</v>
+        <v>917.476365</v>
       </c>
       <c r="E24">
-        <v>0.07590173910164107</v>
+        <v>2332.2831</v>
       </c>
       <c r="F24">
-        <v>0.105454250104877</v>
+        <v>-0.05749951911031789</v>
       </c>
       <c r="G24">
-        <v>0.3839244780239995</v>
+        <v>0.1511009886036988</v>
       </c>
       <c r="H24">
-        <v>0.2619730618214851</v>
+        <v>0.2086005077140167</v>
       </c>
       <c r="I24">
-        <v>0.280240113355746</v>
+        <v>0.03995824281400667</v>
+      </c>
+      <c r="J24">
+        <v>0.3772427726140268</v>
+      </c>
+      <c r="K24">
+        <v>0.01524603902894358</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>neo1</t>
         </is>
       </c>
       <c r="C25">
-        <v>1338</v>
+        <v>768</v>
       </c>
       <c r="D25">
-        <v>1341</v>
+        <v>917.476365</v>
       </c>
       <c r="E25">
-        <v>0.07895195841198628</v>
+        <v>2332.2831</v>
       </c>
       <c r="F25">
-        <v>0.1075606655206243</v>
+        <v>-0.2059476543175023</v>
       </c>
       <c r="G25">
-        <v>0.1103750993742061</v>
+        <v>-0.005424124189817031</v>
       </c>
       <c r="H25">
-        <v>0.2056791428375945</v>
+        <v>0.2005235301276853</v>
       </c>
       <c r="I25">
-        <v>0.2659774088433141</v>
+        <v>0.009938922282632823</v>
+      </c>
+      <c r="J25">
+        <v>0.3911081379727377</v>
+      </c>
+      <c r="K25">
+        <v>0.03886193394109631</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_no4</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>L_conc_t1</t>
         </is>
       </c>
       <c r="C26">
-        <v>1337</v>
+        <v>946</v>
       </c>
       <c r="D26">
-        <v>1340</v>
+        <v>0.21206395</v>
       </c>
       <c r="E26">
-        <v>0.006455079359450477</v>
+        <v>0.9839051</v>
       </c>
       <c r="F26">
-        <v>0.009456386644320134</v>
+        <v>-0.005895299820809848</v>
       </c>
       <c r="G26">
-        <v>0.7659903918888573</v>
+        <v>0.03059114456890792</v>
       </c>
       <c r="H26">
-        <v>0.6646856248062584</v>
+        <v>0.03648644438971776</v>
       </c>
       <c r="I26">
-        <v>0.3173841550432328</v>
+        <v>-0.1936982506663138</v>
+      </c>
+      <c r="J26">
+        <v>0.2666711394457493</v>
+      </c>
+      <c r="K26">
+        <v>0.7688116603615279</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_no4</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>L_conc_t1</t>
         </is>
       </c>
       <c r="C27">
-        <v>1328</v>
+        <v>944</v>
       </c>
       <c r="D27">
-        <v>1340</v>
+        <v>0.211418975</v>
       </c>
       <c r="E27">
-        <v>0.002524776987732523</v>
+        <v>0.9848725749999999</v>
       </c>
       <c r="F27">
-        <v>-1.105176821951289e-10</v>
+        <v>0.1129751624110039</v>
       </c>
       <c r="G27">
-        <v>0.9045864356626154</v>
+        <v>0.1129751623728284</v>
       </c>
       <c r="H27">
-        <v>0.9999710858575335</v>
+        <v>-3.817553734995232e-11</v>
       </c>
       <c r="I27">
-        <v>22845005.86786181</v>
+        <v>-2.171950184052144e-06</v>
+      </c>
+      <c r="J27">
+        <v>2.171873832977445e-06</v>
+      </c>
+      <c r="K27">
+        <v>0.9999752986052546</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_no4</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>L_conc_t1</t>
         </is>
       </c>
       <c r="C28">
-        <v>1331</v>
+        <v>943</v>
       </c>
       <c r="D28">
-        <v>1340</v>
+        <v>0.21103295</v>
       </c>
       <c r="E28">
-        <v>-0.006670166992178135</v>
+        <v>0.9835826</v>
       </c>
       <c r="F28">
-        <v>-0.003543671427216775</v>
+        <v>0.07721856083292672</v>
       </c>
       <c r="G28">
-        <v>0.7427056356476787</v>
+        <v>0.07721947944551182</v>
       </c>
       <c r="H28">
-        <v>0.8692505723144492</v>
+        <v>9.19530603561722e-07</v>
       </c>
       <c r="I28">
-        <v>-0.8822758060887524</v>
+        <v>-1.346717223281928e-06</v>
+      </c>
+      <c r="J28">
+        <v>3.185778430405371e-06</v>
+      </c>
+      <c r="K28">
+        <v>0.4346082352416721</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_no4</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>L_conc_t1</t>
         </is>
       </c>
       <c r="C29">
-        <v>1337</v>
+        <v>944</v>
       </c>
       <c r="D29">
-        <v>1340</v>
+        <v>0.211418975</v>
       </c>
       <c r="E29">
-        <v>-0.006955503614924903</v>
+        <v>0.9832601</v>
       </c>
       <c r="F29">
-        <v>-0.008206060358929689</v>
+        <v>-6.356270976708882e-05</v>
       </c>
       <c r="G29">
-        <v>0.7211265602397594</v>
+        <v>-0.005195340088772183</v>
       </c>
       <c r="H29">
-        <v>0.678626327400139</v>
+        <v>-0.005131777379005095</v>
       </c>
       <c r="I29">
-        <v>0.1523942902325783</v>
+        <v>-0.04880011794803286</v>
+      </c>
+      <c r="J29">
+        <v>0.03853656319002267</v>
+      </c>
+      <c r="K29">
+        <v>0.8292617559056494</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>L_conc_t1</t>
         </is>
       </c>
       <c r="C30">
-        <v>1338</v>
+        <v>948</v>
       </c>
       <c r="D30">
-        <v>1341</v>
+        <v>0.211418975</v>
       </c>
       <c r="E30">
-        <v>0.01143943096516591</v>
+        <v>0.9832601</v>
       </c>
       <c r="F30">
-        <v>0.002976886947639412</v>
+        <v>-0.02650295648627907</v>
       </c>
       <c r="G30">
-        <v>0.6828775636587086</v>
+        <v>0.04382273361656076</v>
       </c>
       <c r="H30">
-        <v>0.9783614367587606</v>
+        <v>0.07032569010283983</v>
       </c>
       <c r="I30">
-        <v>-2.842749545540203</v>
+        <v>-0.1688922479081523</v>
+      </c>
+      <c r="J30">
+        <v>0.309543628113832</v>
+      </c>
+      <c r="K30">
+        <v>0.5762262133322021</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>L_conc_t1</t>
         </is>
       </c>
       <c r="C31">
-        <v>1329</v>
+        <v>948</v>
       </c>
       <c r="D31">
-        <v>1341</v>
+        <v>0.211418975</v>
       </c>
       <c r="E31">
-        <v>0.01409221639535589</v>
+        <v>0.9832601</v>
       </c>
       <c r="F31">
-        <v>0.01246610170402866</v>
+        <v>0.1190109987781155</v>
       </c>
       <c r="G31">
-        <v>0.5880566023286411</v>
+        <v>0.1190109987648936</v>
       </c>
       <c r="H31">
-        <v>0.6415886703284076</v>
+        <v>-1.322182768828083e-11</v>
       </c>
       <c r="I31">
-        <v>-0.1304429187194684</v>
+        <v>-1.772816684255837e-06</v>
+      </c>
+      <c r="J31">
+        <v>1.772790240600461e-06</v>
+      </c>
+      <c r="K31">
+        <v>0.9999895188837933</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>L_conc_t1</t>
         </is>
       </c>
       <c r="C32">
-        <v>1332</v>
+        <v>948</v>
       </c>
       <c r="D32">
-        <v>1341</v>
+        <v>0.211418975</v>
       </c>
       <c r="E32">
-        <v>-0.02121280625055749</v>
+        <v>0.9832601</v>
       </c>
       <c r="F32">
-        <v>-0.0330132215642903</v>
+        <v>-0.03373798640295309</v>
       </c>
       <c r="G32">
-        <v>0.818201335054717</v>
+        <v>0.01672252663753901</v>
       </c>
       <c r="H32">
-        <v>0.7316225840750129</v>
+        <v>0.05046051304049208</v>
       </c>
       <c r="I32">
-        <v>0.3574451312106138</v>
+        <v>-0.1727125222650484</v>
+      </c>
+      <c r="J32">
+        <v>0.2736335483460325</v>
+      </c>
+      <c r="K32">
+        <v>0.6706885987857295</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>L_conc_t1</t>
         </is>
       </c>
       <c r="C33">
-        <v>1338</v>
+        <v>948</v>
       </c>
       <c r="D33">
-        <v>1341</v>
+        <v>0.211418975</v>
       </c>
       <c r="E33">
-        <v>0.003358063174183998</v>
+        <v>0.9832601</v>
       </c>
       <c r="F33">
-        <v>0.03898687467590285</v>
+        <v>-0.1156341456392247</v>
       </c>
       <c r="G33">
-        <v>0.9713296401395324</v>
+        <v>-0.08669281269713955</v>
       </c>
       <c r="H33">
-        <v>0.1153495885751826</v>
+        <v>0.02894133294208512</v>
       </c>
       <c r="I33">
-        <v>0.9138668282056585</v>
+        <v>-0.1838326045377664</v>
+      </c>
+      <c r="J33">
+        <v>0.2417152704219366</v>
+      </c>
+      <c r="K33">
+        <v>0.801943323732609</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_no4</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>L_conc_t2</t>
+          <t>M_conc_t1</t>
         </is>
       </c>
       <c r="C34">
-        <v>1302</v>
+        <v>946</v>
       </c>
       <c r="D34">
-        <v>1305</v>
+        <v>2.0094515</v>
       </c>
       <c r="E34">
-        <v>-0.03904553719836785</v>
+        <v>8.264853499999999</v>
       </c>
       <c r="F34">
-        <v>-0.01632276086875591</v>
+        <v>0.1079218441511242</v>
       </c>
       <c r="G34">
-        <v>0.6242272523372143</v>
+        <v>0.07706962971584981</v>
       </c>
       <c r="H34">
-        <v>0.8337229021764141</v>
+        <v>-0.03085221443527438</v>
       </c>
       <c r="I34">
-        <v>-1.392091479640958</v>
+        <v>-0.07120631382414391</v>
+      </c>
+      <c r="J34">
+        <v>0.009501884953595149</v>
+      </c>
+      <c r="K34">
+        <v>0.1341844510497002</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_no4</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>L_conc_t2</t>
+          <t>M_conc_t1</t>
         </is>
       </c>
       <c r="C35">
-        <v>1297</v>
+        <v>944</v>
       </c>
       <c r="D35">
-        <v>1305</v>
+        <v>2.0060325</v>
       </c>
       <c r="E35">
-        <v>-0.1146235073968982</v>
+        <v>8.2442685</v>
       </c>
       <c r="F35">
-        <v>-0.1027037818111149</v>
+        <v>0.1044424866977154</v>
       </c>
       <c r="G35">
-        <v>0.01956247129909006</v>
+        <v>0.1140629071037656</v>
       </c>
       <c r="H35">
-        <v>0.03613871297173015</v>
+        <v>0.009620420406050234</v>
       </c>
       <c r="I35">
-        <v>-0.1160592665195636</v>
+        <v>-0.02788453588585046</v>
+      </c>
+      <c r="J35">
+        <v>0.04712537669795092</v>
+      </c>
+      <c r="K35">
+        <v>0.6277387371373134</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_no4</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>L_conc_t2</t>
+          <t>M_conc_t1</t>
         </is>
       </c>
       <c r="C36">
-        <v>1297</v>
+        <v>943</v>
       </c>
       <c r="D36">
-        <v>1305</v>
+        <v>2.003224</v>
       </c>
       <c r="E36">
-        <v>-0.1342155867168292</v>
+        <v>8.254560999999999</v>
       </c>
       <c r="F36">
-        <v>-0.1133674371209691</v>
+        <v>0.08114315466035667</v>
       </c>
       <c r="G36">
-        <v>0.0746667472633718</v>
+        <v>0.07685772194672597</v>
       </c>
       <c r="H36">
-        <v>0.1360219679608112</v>
+        <v>-0.004285432713630722</v>
       </c>
       <c r="I36">
-        <v>-0.1838989230533103</v>
+        <v>-0.04294586799628327</v>
+      </c>
+      <c r="J36">
+        <v>0.03437500256902182</v>
+      </c>
+      <c r="K36">
+        <v>0.8391101309721352</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_no4</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>L_conc_t2</t>
+          <t>M_conc_t1</t>
         </is>
       </c>
       <c r="C37">
-        <v>1302</v>
+        <v>944</v>
       </c>
       <c r="D37">
-        <v>1305</v>
+        <v>2.0060325</v>
       </c>
       <c r="E37">
-        <v>-0.08363477992693383</v>
+        <v>8.2912705</v>
       </c>
       <c r="F37">
-        <v>-0.08851008172644707</v>
+        <v>0.007285394038350178</v>
       </c>
       <c r="G37">
-        <v>0.2667579303024778</v>
+        <v>0.09470839230848817</v>
       </c>
       <c r="H37">
-        <v>0.2384751022790607</v>
+        <v>0.08742299827013797</v>
       </c>
       <c r="I37">
-        <v>0.05508188111927244</v>
+        <v>-0.1371194355768482</v>
+      </c>
+      <c r="J37">
+        <v>0.3119654321171242</v>
+      </c>
+      <c r="K37">
+        <v>0.4541203730411344</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>M_conc_t2</t>
+          <t>M_conc_t1</t>
         </is>
       </c>
       <c r="C38">
-        <v>1302</v>
+        <v>948</v>
       </c>
       <c r="D38">
-        <v>1305</v>
+        <v>2.0060325</v>
       </c>
       <c r="E38">
-        <v>-0.06664741160750384</v>
+        <v>8.2442685</v>
       </c>
       <c r="F38">
-        <v>-0.1163942439922983</v>
+        <v>0.1096918193946071</v>
       </c>
       <c r="G38">
-        <v>0.4454264822899703</v>
+        <v>0.08158998353575091</v>
       </c>
       <c r="H38">
-        <v>0.1932864360403027</v>
+        <v>-0.0281018358588562</v>
       </c>
       <c r="I38">
-        <v>0.4273994200957751</v>
+        <v>-0.06917245248175105</v>
+      </c>
+      <c r="J38">
+        <v>0.01296878076403866</v>
+      </c>
+      <c r="K38">
+        <v>0.1809099304725955</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>M_conc_t2</t>
+          <t>M_conc_t1</t>
         </is>
       </c>
       <c r="C39">
-        <v>1297</v>
+        <v>948</v>
       </c>
       <c r="D39">
-        <v>1305</v>
+        <v>2.0060325</v>
       </c>
       <c r="E39">
-        <v>-0.05484865216214484</v>
+        <v>8.2442685</v>
       </c>
       <c r="F39">
-        <v>-0.2109059370113006</v>
+        <v>0.1088340122304826</v>
       </c>
       <c r="G39">
-        <v>0.1392139934717748</v>
+        <v>0.1203206052402771</v>
       </c>
       <c r="H39">
-        <v>0.004916357007366671</v>
+        <v>0.0114865930097945</v>
       </c>
       <c r="I39">
-        <v>0.7399378465139841</v>
+        <v>-0.0246944153917832</v>
+      </c>
+      <c r="J39">
+        <v>0.04766760141137219</v>
+      </c>
+      <c r="K39">
+        <v>0.5448583309930062</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>combined</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>M_conc_t2</t>
+          <t>M_conc_t1</t>
         </is>
       </c>
       <c r="C40">
-        <v>1297</v>
+        <v>948</v>
       </c>
       <c r="D40">
-        <v>1305</v>
+        <v>2.0060325</v>
       </c>
       <c r="E40">
-        <v>0.01360971707537369</v>
+        <v>8.2442685</v>
       </c>
       <c r="F40">
-        <v>-0.1299850267047005</v>
+        <v>0.06653234657542602</v>
       </c>
       <c r="G40">
-        <v>0.5559063939360782</v>
+        <v>0.06616456631803866</v>
       </c>
       <c r="H40">
-        <v>0.1082799889872837</v>
+        <v>-0.0003677802573873289</v>
       </c>
       <c r="I40">
-        <v>1.104702190863046</v>
+        <v>-0.03959848806342327</v>
+      </c>
+      <c r="J40">
+        <v>0.03886292754864861</v>
+      </c>
+      <c r="K40">
+        <v>0.986773198790769</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>M_conc_t1</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>948</v>
+      </c>
+      <c r="D41">
+        <v>2.0060325</v>
+      </c>
+      <c r="E41">
+        <v>8.2442685</v>
+      </c>
+      <c r="F41">
+        <v>-0.04260893563755792</v>
+      </c>
+      <c r="G41">
+        <v>-0.03304455047307499</v>
+      </c>
+      <c r="H41">
+        <v>0.009564385164482917</v>
+      </c>
+      <c r="I41">
+        <v>-0.02837804137691621</v>
+      </c>
+      <c r="J41">
+        <v>0.04750681170588204</v>
+      </c>
+      <c r="K41">
+        <v>0.6339435596472874</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_no4</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>aat2</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>1338</v>
+      </c>
+      <c r="D42">
+        <v>0.25412755</v>
+      </c>
+      <c r="E42">
+        <v>0.889681175</v>
+      </c>
+      <c r="F42">
+        <v>0.1099673327950801</v>
+      </c>
+      <c r="G42">
+        <v>0.2669274840196936</v>
+      </c>
+      <c r="H42">
+        <v>0.1569601512246135</v>
+      </c>
+      <c r="I42">
+        <v>-0.02611861227876405</v>
+      </c>
+      <c r="J42">
+        <v>0.340038914727991</v>
+      </c>
+      <c r="K42">
+        <v>0.09259852070261805</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_no4</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>aat2</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>1329</v>
+      </c>
+      <c r="D43">
+        <v>0.2532013</v>
+      </c>
+      <c r="E43">
+        <v>0.888563</v>
+      </c>
+      <c r="F43">
+        <v>0.1213647202325969</v>
+      </c>
+      <c r="G43">
+        <v>0.1862439009931828</v>
+      </c>
+      <c r="H43">
+        <v>0.06487918076058591</v>
+      </c>
+      <c r="I43">
+        <v>-0.120929256097763</v>
+      </c>
+      <c r="J43">
+        <v>0.2506876176189349</v>
+      </c>
+      <c r="K43">
+        <v>0.5038169794530788</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_no4</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>aat2</t>
+        </is>
+      </c>
+      <c r="C44">
+        <v>1332</v>
+      </c>
+      <c r="D44">
+        <v>0.25420985</v>
+      </c>
+      <c r="E44">
+        <v>0.891273675</v>
+      </c>
+      <c r="F44">
+        <v>0.09345800622509902</v>
+      </c>
+      <c r="G44">
+        <v>0.1693597453267401</v>
+      </c>
+      <c r="H44">
+        <v>0.07590173910164107</v>
+      </c>
+      <c r="I44">
+        <v>-0.09259778114957566</v>
+      </c>
+      <c r="J44">
+        <v>0.2444012593528578</v>
+      </c>
+      <c r="K44">
+        <v>0.3839244780239995</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_no4</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>aat2</t>
+        </is>
+      </c>
+      <c r="C45">
+        <v>1338</v>
+      </c>
+      <c r="D45">
+        <v>0.254496125</v>
+      </c>
+      <c r="E45">
+        <v>0.8937132249999999</v>
+      </c>
+      <c r="F45">
+        <v>0.04215199010808558</v>
+      </c>
+      <c r="G45">
+        <v>0.1211039485200719</v>
+      </c>
+      <c r="H45">
+        <v>0.07895195841198628</v>
+      </c>
+      <c r="I45">
+        <v>-0.01800965120333048</v>
+      </c>
+      <c r="J45">
+        <v>0.175913568027303</v>
+      </c>
+      <c r="K45">
+        <v>0.1103750993742061</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_all</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>aat2</t>
+        </is>
+      </c>
+      <c r="C46">
+        <v>1341</v>
+      </c>
+      <c r="D46">
+        <v>0.2540864</v>
+      </c>
+      <c r="E46">
+        <v>0.8900539</v>
+      </c>
+      <c r="F46">
+        <v>0.1002249340798554</v>
+      </c>
+      <c r="G46">
+        <v>0.2502921939749468</v>
+      </c>
+      <c r="H46">
+        <v>0.1500672598950913</v>
+      </c>
+      <c r="I46">
+        <v>-0.03872999422696269</v>
+      </c>
+      <c r="J46">
+        <v>0.3388645140171453</v>
+      </c>
+      <c r="K46">
+        <v>0.119228075809969</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_all</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>aat2</t>
+        </is>
+      </c>
+      <c r="C47">
+        <v>1341</v>
+      </c>
+      <c r="D47">
+        <v>0.2540864</v>
+      </c>
+      <c r="E47">
+        <v>0.8900539</v>
+      </c>
+      <c r="F47">
+        <v>0.1124568088105909</v>
+      </c>
+      <c r="G47">
+        <v>0.09738654401318594</v>
+      </c>
+      <c r="H47">
+        <v>-0.01507026479740493</v>
+      </c>
+      <c r="I47">
+        <v>-0.08150408702417232</v>
+      </c>
+      <c r="J47">
+        <v>0.05136355742936245</v>
+      </c>
+      <c r="K47">
+        <v>0.669630718554056</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_all</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>aat2</t>
+        </is>
+      </c>
+      <c r="C48">
+        <v>1341</v>
+      </c>
+      <c r="D48">
+        <v>0.2540864</v>
+      </c>
+      <c r="E48">
+        <v>0.8900539</v>
+      </c>
+      <c r="F48">
+        <v>0.1090804302353372</v>
+      </c>
+      <c r="G48">
+        <v>0.2145346803402142</v>
+      </c>
+      <c r="H48">
+        <v>0.105454250104877</v>
+      </c>
+      <c r="I48">
+        <v>-0.07764208516258224</v>
+      </c>
+      <c r="J48">
+        <v>0.2885505853723362</v>
+      </c>
+      <c r="K48">
+        <v>0.2619730618214851</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_all</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>aat2</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>1341</v>
+      </c>
+      <c r="D49">
+        <v>0.2540864</v>
+      </c>
+      <c r="E49">
+        <v>0.8900539</v>
+      </c>
+      <c r="F49">
+        <v>0.04027941499515678</v>
+      </c>
+      <c r="G49">
+        <v>0.1478400805157811</v>
+      </c>
+      <c r="H49">
+        <v>0.1075606655206243</v>
+      </c>
+      <c r="I49">
+        <v>-0.0584472064610992</v>
+      </c>
+      <c r="J49">
+        <v>0.2735685375023479</v>
+      </c>
+      <c r="K49">
+        <v>0.2056791428375945</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_no4</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>mpo2</t>
+        </is>
+      </c>
+      <c r="C50">
+        <v>1337</v>
+      </c>
+      <c r="D50">
+        <v>2731.177</v>
+      </c>
+      <c r="E50">
+        <v>10322.586</v>
+      </c>
+      <c r="F50">
+        <v>0.1553880788489112</v>
+      </c>
+      <c r="G50">
+        <v>0.1618431582083617</v>
+      </c>
+      <c r="H50">
+        <v>0.006455079359450477</v>
+      </c>
+      <c r="I50">
+        <v>-0.03378123256838825</v>
+      </c>
+      <c r="J50">
+        <v>0.04669139128728921</v>
+      </c>
+      <c r="K50">
+        <v>0.7659903918888573</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_no4</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>mpo2</t>
+        </is>
+      </c>
+      <c r="C51">
+        <v>1328</v>
+      </c>
+      <c r="D51">
+        <v>2726.6665</v>
+      </c>
+      <c r="E51">
+        <v>10319.42625</v>
+      </c>
+      <c r="F51">
+        <v>0.119227685147151</v>
+      </c>
+      <c r="G51">
+        <v>0.1217524621348836</v>
+      </c>
+      <c r="H51">
+        <v>0.002524776987732523</v>
+      </c>
+      <c r="I51">
+        <v>-0.03552796054043399</v>
+      </c>
+      <c r="J51">
+        <v>0.04057751451589903</v>
+      </c>
+      <c r="K51">
+        <v>0.9045864356626154</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_no4</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>mpo2</t>
+        </is>
+      </c>
+      <c r="C52">
+        <v>1331</v>
+      </c>
+      <c r="D52">
+        <v>2728.487</v>
+      </c>
+      <c r="E52">
+        <v>10315.122</v>
+      </c>
+      <c r="F52">
+        <v>0.1043681625887946</v>
+      </c>
+      <c r="G52">
+        <v>0.09769799559661645</v>
+      </c>
+      <c r="H52">
+        <v>-0.006670166992178135</v>
+      </c>
+      <c r="I52">
+        <v>-0.0445015456634254</v>
+      </c>
+      <c r="J52">
+        <v>0.03116121167906913</v>
+      </c>
+      <c r="K52">
+        <v>0.7427056356476787</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_no4</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>mpo2</t>
+        </is>
+      </c>
+      <c r="C53">
+        <v>1337</v>
+      </c>
+      <c r="D53">
+        <v>2731.177</v>
+      </c>
+      <c r="E53">
+        <v>10311.871</v>
+      </c>
+      <c r="F53">
+        <v>0.06098360756255437</v>
+      </c>
+      <c r="G53">
+        <v>0.05402810394762947</v>
+      </c>
+      <c r="H53">
+        <v>-0.006955503614924903</v>
+      </c>
+      <c r="I53">
+        <v>-0.04335057922513252</v>
+      </c>
+      <c r="J53">
+        <v>0.02943957199528271</v>
+      </c>
+      <c r="K53">
+        <v>0.7211265602397594</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_all</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>mpo2</t>
+        </is>
+      </c>
+      <c r="C54">
+        <v>1340</v>
+      </c>
+      <c r="D54">
+        <v>2730.59025</v>
+      </c>
+      <c r="E54">
+        <v>10319.42625</v>
+      </c>
+      <c r="F54">
+        <v>0.1462041490430123</v>
+      </c>
+      <c r="G54">
+        <v>0.1556605356873325</v>
+      </c>
+      <c r="H54">
+        <v>0.009456386644320134</v>
+      </c>
+      <c r="I54">
+        <v>-0.03160183017880359</v>
+      </c>
+      <c r="J54">
+        <v>0.05051460346744387</v>
+      </c>
+      <c r="K54">
+        <v>0.6646856248062584</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_all</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>mpo2</t>
+        </is>
+      </c>
+      <c r="C55">
+        <v>1340</v>
+      </c>
+      <c r="D55">
+        <v>2730.59025</v>
+      </c>
+      <c r="E55">
+        <v>10319.42625</v>
+      </c>
+      <c r="F55">
+        <v>0.1018980596883846</v>
+      </c>
+      <c r="G55">
+        <v>0.1018980595778669</v>
+      </c>
+      <c r="H55">
+        <v>-1.105176821951289e-10</v>
+      </c>
+      <c r="I55">
+        <v>-5.371672124749506e-06</v>
+      </c>
+      <c r="J55">
+        <v>5.371451089385115e-06</v>
+      </c>
+      <c r="K55">
+        <v>0.9999710858575335</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_all</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>mpo2</t>
+        </is>
+      </c>
+      <c r="C56">
+        <v>1340</v>
+      </c>
+      <c r="D56">
+        <v>2730.59025</v>
+      </c>
+      <c r="E56">
+        <v>10319.42625</v>
+      </c>
+      <c r="F56">
+        <v>0.1074711760319053</v>
+      </c>
+      <c r="G56">
+        <v>0.1039275046046885</v>
+      </c>
+      <c r="H56">
+        <v>-0.003543671427216775</v>
+      </c>
+      <c r="I56">
+        <v>-0.04273770449990458</v>
+      </c>
+      <c r="J56">
+        <v>0.03565036164547104</v>
+      </c>
+      <c r="K56">
+        <v>0.8692505723144492</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_all</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>mpo2</t>
+        </is>
+      </c>
+      <c r="C57">
+        <v>1340</v>
+      </c>
+      <c r="D57">
+        <v>2730.59025</v>
+      </c>
+      <c r="E57">
+        <v>10319.42625</v>
+      </c>
+      <c r="F57">
+        <v>0.04649193169989694</v>
+      </c>
+      <c r="G57">
+        <v>0.03828587134096724</v>
+      </c>
+      <c r="H57">
+        <v>-0.008206060358929689</v>
+      </c>
+      <c r="I57">
+        <v>-0.04541285540703061</v>
+      </c>
+      <c r="J57">
+        <v>0.02900073468917122</v>
+      </c>
+      <c r="K57">
+        <v>0.678626327400139</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_no4</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>neo2</t>
+        </is>
+      </c>
+      <c r="C58">
+        <v>1338</v>
+      </c>
+      <c r="D58">
+        <v>648.7747499999999</v>
+      </c>
+      <c r="E58">
+        <v>2078.04175</v>
+      </c>
+      <c r="F58">
+        <v>0.1598160670496528</v>
+      </c>
+      <c r="G58">
+        <v>0.1712554980148188</v>
+      </c>
+      <c r="H58">
+        <v>0.01143943096516591</v>
+      </c>
+      <c r="I58">
+        <v>-0.04113468644453911</v>
+      </c>
+      <c r="J58">
+        <v>0.06401354837487093</v>
+      </c>
+      <c r="K58">
+        <v>0.6828775636587086</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_no4</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>neo2</t>
+        </is>
+      </c>
+      <c r="C59">
+        <v>1329</v>
+      </c>
+      <c r="D59">
+        <v>648.766</v>
+      </c>
+      <c r="E59">
+        <v>2082.658</v>
+      </c>
+      <c r="F59">
+        <v>0.1109433929148274</v>
+      </c>
+      <c r="G59">
+        <v>0.1250356093101833</v>
+      </c>
+      <c r="H59">
+        <v>0.01409221639535589</v>
+      </c>
+      <c r="I59">
+        <v>-0.03530853483722517</v>
+      </c>
+      <c r="J59">
+        <v>0.06349296762793696</v>
+      </c>
+      <c r="K59">
+        <v>0.5880566023286411</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_no4</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>neo2</t>
+        </is>
+      </c>
+      <c r="C60">
+        <v>1332</v>
+      </c>
+      <c r="D60">
+        <v>648.7922500000001</v>
+      </c>
+      <c r="E60">
+        <v>2079.89725</v>
+      </c>
+      <c r="F60">
+        <v>0.131986508046903</v>
+      </c>
+      <c r="G60">
+        <v>0.1107737017963455</v>
+      </c>
+      <c r="H60">
+        <v>-0.02121280625055749</v>
+      </c>
+      <c r="I60">
+        <v>-0.1909066501350602</v>
+      </c>
+      <c r="J60">
+        <v>0.1484810376339452</v>
+      </c>
+      <c r="K60">
+        <v>0.818201335054717</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_no4</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>neo2</t>
+        </is>
+      </c>
+      <c r="C61">
+        <v>1338</v>
+      </c>
+      <c r="D61">
+        <v>649.2840000000001</v>
+      </c>
+      <c r="E61">
+        <v>2078.04175</v>
+      </c>
+      <c r="F61">
+        <v>0.0778719373055696</v>
+      </c>
+      <c r="G61">
+        <v>0.08123000047975362</v>
+      </c>
+      <c r="H61">
+        <v>0.003358063174183998</v>
+      </c>
+      <c r="I61">
+        <v>-0.1626041828894163</v>
+      </c>
+      <c r="J61">
+        <v>0.1693203092377843</v>
+      </c>
+      <c r="K61">
+        <v>0.9713296401395324</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_all</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>neo2</t>
+        </is>
+      </c>
+      <c r="C62">
+        <v>1341</v>
+      </c>
+      <c r="D62">
+        <v>648.766</v>
+      </c>
+      <c r="E62">
+        <v>2078.977</v>
+      </c>
+      <c r="F62">
+        <v>0.171218894283864</v>
+      </c>
+      <c r="G62">
+        <v>0.1741957812315034</v>
+      </c>
+      <c r="H62">
+        <v>0.002976886947639412</v>
+      </c>
+      <c r="I62">
+        <v>-0.1915855231395192</v>
+      </c>
+      <c r="J62">
+        <v>0.1975392970347981</v>
+      </c>
+      <c r="K62">
+        <v>0.9783614367587606</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_all</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>neo2</t>
+        </is>
+      </c>
+      <c r="C63">
+        <v>1341</v>
+      </c>
+      <c r="D63">
+        <v>648.766</v>
+      </c>
+      <c r="E63">
+        <v>2078.977</v>
+      </c>
+      <c r="F63">
+        <v>0.09281955664873601</v>
+      </c>
+      <c r="G63">
+        <v>0.1052856583527647</v>
+      </c>
+      <c r="H63">
+        <v>0.01246610170402866</v>
+      </c>
+      <c r="I63">
+        <v>-0.03807902035991332</v>
+      </c>
+      <c r="J63">
+        <v>0.06301122376797064</v>
+      </c>
+      <c r="K63">
+        <v>0.6415886703284076</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_all</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>neo2</t>
+        </is>
+      </c>
+      <c r="C64">
+        <v>1341</v>
+      </c>
+      <c r="D64">
+        <v>648.766</v>
+      </c>
+      <c r="E64">
+        <v>2078.977</v>
+      </c>
+      <c r="F64">
+        <v>0.1440937291238849</v>
+      </c>
+      <c r="G64">
+        <v>0.1110805075595946</v>
+      </c>
+      <c r="H64">
+        <v>-0.0330132215642903</v>
+      </c>
+      <c r="I64">
+        <v>-0.2125277854445705</v>
+      </c>
+      <c r="J64">
+        <v>0.1465013423159898</v>
+      </c>
+      <c r="K64">
+        <v>0.7316225840750129</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_all</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>neo2</t>
+        </is>
+      </c>
+      <c r="C65">
+        <v>1341</v>
+      </c>
+      <c r="D65">
+        <v>648.766</v>
+      </c>
+      <c r="E65">
+        <v>2078.977</v>
+      </c>
+      <c r="F65">
+        <v>0.0229776047665771</v>
+      </c>
+      <c r="G65">
+        <v>0.06196447944247994</v>
+      </c>
+      <c r="H65">
+        <v>0.03898687467590285</v>
+      </c>
+      <c r="I65">
+        <v>-0.009551821790859921</v>
+      </c>
+      <c r="J65">
+        <v>0.08752557114266561</v>
+      </c>
+      <c r="K65">
+        <v>0.1153495885751826</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_no4</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>L_conc_t2</t>
+        </is>
+      </c>
+      <c r="C66">
+        <v>1302</v>
+      </c>
+      <c r="D66">
+        <v>0.146860175</v>
+      </c>
+      <c r="E66">
+        <v>0.5959701500000001</v>
+      </c>
+      <c r="F66">
+        <v>0.1928129574016766</v>
+      </c>
+      <c r="G66">
+        <v>0.1537674202033088</v>
+      </c>
+      <c r="H66">
+        <v>-0.03904553719836785</v>
+      </c>
+      <c r="I66">
+        <v>-0.1897847687601809</v>
+      </c>
+      <c r="J66">
+        <v>0.1116936943634452</v>
+      </c>
+      <c r="K66">
+        <v>0.6242272523372143</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_no4</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>L_conc_t2</t>
+        </is>
+      </c>
+      <c r="C67">
+        <v>1297</v>
+      </c>
+      <c r="D67">
+        <v>0.1478276</v>
+      </c>
+      <c r="E67">
+        <v>0.5933744</v>
+      </c>
+      <c r="F67">
+        <v>0.1857905896178314</v>
+      </c>
+      <c r="G67">
+        <v>0.07116708222093321</v>
+      </c>
+      <c r="H67">
+        <v>-0.1146235073968982</v>
+      </c>
+      <c r="I67">
+        <v>-0.210965459059574</v>
+      </c>
+      <c r="J67">
+        <v>-0.0182815557342224</v>
+      </c>
+      <c r="K67">
+        <v>0.01956247129909006</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_no4</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>L_conc_t2</t>
+        </is>
+      </c>
+      <c r="C68">
+        <v>1297</v>
+      </c>
+      <c r="D68">
+        <v>0.1478276</v>
+      </c>
+      <c r="E68">
+        <v>0.5959544</v>
+      </c>
+      <c r="F68">
+        <v>0.1818830165910699</v>
+      </c>
+      <c r="G68">
+        <v>0.04766742987424076</v>
+      </c>
+      <c r="H68">
+        <v>-0.1342155867168292</v>
+      </c>
+      <c r="I68">
+        <v>-0.2819882004239701</v>
+      </c>
+      <c r="J68">
+        <v>0.01355702699031167</v>
+      </c>
+      <c r="K68">
+        <v>0.0746667472633718</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_no4</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>L_conc_t2</t>
+        </is>
+      </c>
+      <c r="C69">
+        <v>1302</v>
+      </c>
+      <c r="D69">
+        <v>0.146860175</v>
+      </c>
+      <c r="E69">
+        <v>0.5959701500000001</v>
+      </c>
+      <c r="F69">
+        <v>0.09436903677868781</v>
+      </c>
+      <c r="G69">
+        <v>0.01073425685175397</v>
+      </c>
+      <c r="H69">
+        <v>-0.08363477992693383</v>
+      </c>
+      <c r="I69">
+        <v>-0.2302702692361479</v>
+      </c>
+      <c r="J69">
+        <v>0.06300070938228028</v>
+      </c>
+      <c r="K69">
+        <v>0.2667579303024778</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_all</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>L_conc_t2</t>
+        </is>
+      </c>
+      <c r="C70">
+        <v>1305</v>
+      </c>
+      <c r="D70">
+        <v>0.1478276</v>
+      </c>
+      <c r="E70">
+        <v>0.5959544</v>
+      </c>
+      <c r="F70">
+        <v>0.1733247355457942</v>
+      </c>
+      <c r="G70">
+        <v>0.1570019746770383</v>
+      </c>
+      <c r="H70">
+        <v>-0.01632276086875591</v>
+      </c>
+      <c r="I70">
+        <v>-0.1588842077942463</v>
+      </c>
+      <c r="J70">
+        <v>0.1262386860567345</v>
+      </c>
+      <c r="K70">
+        <v>0.8337229021764141</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_all</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>L_conc_t2</t>
+        </is>
+      </c>
+      <c r="C71">
+        <v>1305</v>
+      </c>
+      <c r="D71">
+        <v>0.1478276</v>
+      </c>
+      <c r="E71">
+        <v>0.5959544</v>
+      </c>
+      <c r="F71">
+        <v>0.1692909907321464</v>
+      </c>
+      <c r="G71">
+        <v>0.06658720892103155</v>
+      </c>
+      <c r="H71">
+        <v>-0.1027037818111149</v>
+      </c>
+      <c r="I71">
+        <v>-0.1989306245997795</v>
+      </c>
+      <c r="J71">
+        <v>-0.006476939022450307</v>
+      </c>
+      <c r="K71">
+        <v>0.03613871297173015</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_all</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>L_conc_t2</t>
+        </is>
+      </c>
+      <c r="C72">
+        <v>1305</v>
+      </c>
+      <c r="D72">
+        <v>0.1478276</v>
+      </c>
+      <c r="E72">
+        <v>0.5959544</v>
+      </c>
+      <c r="F72">
+        <v>0.1794890837464025</v>
+      </c>
+      <c r="G72">
+        <v>0.06612164662543342</v>
+      </c>
+      <c r="H72">
+        <v>-0.1133674371209691</v>
+      </c>
+      <c r="I72">
+        <v>-0.2623394162133708</v>
+      </c>
+      <c r="J72">
+        <v>0.03560454197143259</v>
+      </c>
+      <c r="K72">
+        <v>0.1360219679608112</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_all</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>L_conc_t2</t>
+        </is>
+      </c>
+      <c r="C73">
+        <v>1305</v>
+      </c>
+      <c r="D73">
+        <v>0.1478276</v>
+      </c>
+      <c r="E73">
+        <v>0.5959544</v>
+      </c>
+      <c r="F73">
+        <v>0.0800577479807964</v>
+      </c>
+      <c r="G73">
+        <v>-0.008452333745650674</v>
+      </c>
+      <c r="H73">
+        <v>-0.08851008172644707</v>
+      </c>
+      <c r="I73">
+        <v>-0.2349291598226859</v>
+      </c>
+      <c r="J73">
+        <v>0.05790899636979173</v>
+      </c>
+      <c r="K73">
+        <v>0.2384751022790607</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_no4</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>M_conc_t2</t>
         </is>
       </c>
-      <c r="C41">
+      <c r="C74">
         <v>1302</v>
       </c>
-      <c r="D41">
+      <c r="D74">
+        <v>1.026887</v>
+      </c>
+      <c r="E74">
+        <v>4.680760250000001</v>
+      </c>
+      <c r="F74">
+        <v>0.1612128197601656</v>
+      </c>
+      <c r="G74">
+        <v>0.09448951974349599</v>
+      </c>
+      <c r="H74">
+        <v>-0.06664741160750384</v>
+      </c>
+      <c r="I74">
+        <v>-0.234693604968722</v>
+      </c>
+      <c r="J74">
+        <v>0.1013987817537143</v>
+      </c>
+      <c r="K74">
+        <v>0.4454264822899703</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_no4</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>M_conc_t2</t>
+        </is>
+      </c>
+      <c r="C75">
+        <v>1297</v>
+      </c>
+      <c r="D75">
+        <v>1.03055</v>
+      </c>
+      <c r="E75">
+        <v>4.683877</v>
+      </c>
+      <c r="F75">
+        <v>0.166017723463751</v>
+      </c>
+      <c r="G75">
+        <v>0.1111690713016062</v>
+      </c>
+      <c r="H75">
+        <v>-0.05484865216214484</v>
+      </c>
+      <c r="I75">
+        <v>-0.1275017641266625</v>
+      </c>
+      <c r="J75">
+        <v>0.01780445980237285</v>
+      </c>
+      <c r="K75">
+        <v>0.1392139934717748</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_no4</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>M_conc_t2</t>
+        </is>
+      </c>
+      <c r="C76">
+        <v>1297</v>
+      </c>
+      <c r="D76">
+        <v>1.03055</v>
+      </c>
+      <c r="E76">
+        <v>4.683877</v>
+      </c>
+      <c r="F76">
+        <v>0.09942930714162043</v>
+      </c>
+      <c r="G76">
+        <v>0.1130390242169941</v>
+      </c>
+      <c r="H76">
+        <v>0.01360971707537369</v>
+      </c>
+      <c r="I76">
+        <v>-0.03041545967783975</v>
+      </c>
+      <c r="J76">
+        <v>0.05763489382858712</v>
+      </c>
+      <c r="K76">
+        <v>0.5559063939360782</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_no4</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>M_conc_t2</t>
+        </is>
+      </c>
+      <c r="C77">
+        <v>1302</v>
+      </c>
+      <c r="D77">
+        <v>1.026887</v>
+      </c>
+      <c r="E77">
+        <v>4.680760250000001</v>
+      </c>
+      <c r="F77">
+        <v>0.03804042990782174</v>
+      </c>
+      <c r="G77">
+        <v>0.03458137753532114</v>
+      </c>
+      <c r="H77">
+        <v>-0.003347583861889903</v>
+      </c>
+      <c r="I77">
+        <v>-0.1431816165787549</v>
+      </c>
+      <c r="J77">
+        <v>0.1364864488549751</v>
+      </c>
+      <c r="K77">
+        <v>0.9660315175715569</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>z_age2mo_personal_all</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>M_conc_t2</t>
+        </is>
+      </c>
+      <c r="C78">
         <v>1305</v>
       </c>
-      <c r="E41">
-        <v>-0.003347583861889903</v>
-      </c>
-      <c r="F41">
+      <c r="D78">
+        <v>1.03055</v>
+      </c>
+      <c r="E78">
+        <v>4.683877</v>
+      </c>
+      <c r="F78">
+        <v>0.1605900660892191</v>
+      </c>
+      <c r="G78">
+        <v>0.04419582209692079</v>
+      </c>
+      <c r="H78">
+        <v>-0.1163942439922983</v>
+      </c>
+      <c r="I78">
+        <v>-0.2912503113734057</v>
+      </c>
+      <c r="J78">
+        <v>0.05846182338880916</v>
+      </c>
+      <c r="K78">
+        <v>0.1932864360403027</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>z_age2mo_motor_all</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>M_conc_t2</t>
+        </is>
+      </c>
+      <c r="C79">
+        <v>1305</v>
+      </c>
+      <c r="D79">
+        <v>1.03055</v>
+      </c>
+      <c r="E79">
+        <v>4.683877</v>
+      </c>
+      <c r="F79">
+        <v>0.2032466613805519</v>
+      </c>
+      <c r="G79">
+        <v>-0.007659275630748693</v>
+      </c>
+      <c r="H79">
+        <v>-0.2109059370113006</v>
+      </c>
+      <c r="I79">
+        <v>-0.3577473588514867</v>
+      </c>
+      <c r="J79">
+        <v>-0.06406451517111447</v>
+      </c>
+      <c r="K79">
+        <v>0.004916357007366671</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>z_age2mo_combined_all</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>M_conc_t2</t>
+        </is>
+      </c>
+      <c r="C80">
+        <v>1305</v>
+      </c>
+      <c r="D80">
+        <v>1.03055</v>
+      </c>
+      <c r="E80">
+        <v>4.683877</v>
+      </c>
+      <c r="F80">
+        <v>0.1619622299008563</v>
+      </c>
+      <c r="G80">
+        <v>0.03197720319615588</v>
+      </c>
+      <c r="H80">
+        <v>-0.1299850267047005</v>
+      </c>
+      <c r="I80">
+        <v>-0.2886905967133016</v>
+      </c>
+      <c r="J80">
+        <v>0.02872054330390059</v>
+      </c>
+      <c r="K80">
+        <v>0.1082799889872837</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>z_age2mo_com_all</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>M_conc_t2</t>
+        </is>
+      </c>
+      <c r="C81">
+        <v>1305</v>
+      </c>
+      <c r="D81">
+        <v>1.03055</v>
+      </c>
+      <c r="E81">
+        <v>4.683877</v>
+      </c>
+      <c r="F81">
+        <v>0.01850519644281663</v>
+      </c>
+      <c r="G81">
+        <v>0.04027666471325936</v>
+      </c>
+      <c r="H81">
         <v>0.02177146827044273</v>
       </c>
-      <c r="G41">
-        <v>0.9660315175715569</v>
-      </c>
-      <c r="H41">
+      <c r="I81">
+        <v>-0.02122728404632909</v>
+      </c>
+      <c r="J81">
+        <v>0.06477022058721454</v>
+      </c>
+      <c r="K81">
         <v>0.3258703127825445</v>
-      </c>
-      <c r="I41">
-        <v>1.153760133230639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>